<commit_message>
fixed duplicate in fastq 3275
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_3275.xlsx
+++ b/fastqFiles/fastq_3275.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E21643-80D6-5B43-84CD-FAD6763C32D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1E9F6C-BB0B-804C-BDCF-2B15B6F59770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14820" yWindow="1040" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14820" yWindow="1040" windowWidth="16100" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="45">
   <si>
     <t>libraryDate</t>
   </si>
@@ -213,11 +213,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E12"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -644,23 +645,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>3275</v>
-      </c>
-      <c r="E5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D5" s="2">
+        <v>3275</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1212,7 +1213,7 @@
         <v>43</v>
       </c>
       <c r="C33">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D33">
         <v>3275</v>
@@ -1221,7 +1222,7 @@
         <v>44</v>
       </c>
       <c r="F33" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1232,7 +1233,7 @@
         <v>43</v>
       </c>
       <c r="C34">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D34">
         <v>3275</v>
@@ -1241,26 +1242,6 @@
         <v>44</v>
       </c>
       <c r="F34" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35">
-        <v>34</v>
-      </c>
-      <c r="D35">
-        <v>3275</v>
-      </c>
-      <c r="E35" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>